<commit_message>
Improved upon database querying when exporting model
Query code is now shorter and more legible. Queries now handle null values more effectively.
</commit_message>
<xml_diff>
--- a/DataFiles/REMS2020_ExampleA_2_Experiments.xlsx
+++ b/DataFiles/REMS2020_ExampleA_2_Experiments.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmstow1\Documents\REMS - Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmstow1\Documents\GitHub\REMS2020\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="270" yWindow="660" windowWidth="15480" windowHeight="4755" tabRatio="669" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="270" yWindow="660" windowWidth="15480" windowHeight="4755" tabRatio="669" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="20" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Notes</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>RepetitionNumber</t>
   </si>
 </sst>
 </file>
@@ -721,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -3233,8 +3236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3250,7 +3253,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>20</v>

</xml_diff>